<commit_message>
[kbss-cvut/termit-ui#449] Fix broken test (change of delimiter from , to ;)
</commit_message>
<xml_diff>
--- a/src/test/resources/data/import-with-plural-atts-en-cs.xlsx
+++ b/src/test/resources/data/import-with-plural-atts-en-cs.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="English" sheetId="1" state="visible" r:id="rId2"/>
@@ -72,7 +72,7 @@
     <t xml:space="preserve">Building</t>
   </si>
   <si>
-    <t xml:space="preserve">Structure, House</t>
+    <t xml:space="preserve">Structure; House</t>
   </si>
   <si>
     <t xml:space="preserve">bldng</t>
@@ -141,7 +141,7 @@
     <t xml:space="preserve">Budova</t>
   </si>
   <si>
-    <t xml:space="preserve">dům, stavba</t>
+    <t xml:space="preserve">dům; stavba</t>
   </si>
   <si>
     <t xml:space="preserve">barák</t>
@@ -304,11 +304,11 @@
   </sheetPr>
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
@@ -17390,11 +17390,11 @@
   </sheetPr>
   <dimension ref="A1:O1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N3" activeCellId="0" sqref="N3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="16.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.5"/>
@@ -34476,7 +34476,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="75.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.37"/>

</xml_diff>